<commit_message>
3a3 uploading some geometric results
</commit_message>
<xml_diff>
--- a/IIA/3A3/Compressor_Lab/compressor_data.xlsx
+++ b/IIA/3A3/Compressor_Lab/compressor_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\MEng-CW\IIA\3A3\Compressor_Lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\source\repos\MEng-CW\IIA\3A3\Compressor_Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F312B1E-7588-48DA-9FAD-3AAC0936BAE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31C0097-85A7-4E4D-9BF7-87334EE383AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" xr2:uid="{02A5341C-B6F3-4355-81FB-8A9D87FE953C}"/>
+    <workbookView xWindow="4538" yWindow="1965" windowWidth="21599" windowHeight="11333" xr2:uid="{02A5341C-B6F3-4355-81FB-8A9D87FE953C}"/>
   </bookViews>
   <sheets>
     <sheet name="preface" sheetId="6" r:id="rId1"/>
@@ -501,24 +501,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE3641E-77F1-44E2-8594-EE5188095FA3}">
   <dimension ref="A4:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="5" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -529,7 +529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -540,7 +540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -551,7 +551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -562,12 +562,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -578,8 +578,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="16" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -588,7 +588,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -599,7 +599,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -607,16 +607,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2142626B-EBBF-4FEB-9B54-0EED73F66AB9}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="26.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,7 +630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2">
         <v>20.7</v>
       </c>
@@ -644,7 +644,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2">
         <v>20.2</v>
       </c>
@@ -658,7 +658,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2">
         <v>19.2</v>
       </c>
@@ -672,7 +672,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
         <v>18.100000000000001</v>
       </c>
@@ -686,7 +686,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2">
         <v>15.7</v>
       </c>
@@ -700,7 +700,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
         <v>12.2</v>
       </c>
@@ -714,7 +714,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2">
         <v>9.8000000000000007</v>
       </c>
@@ -728,7 +728,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="2">
         <v>6.6</v>
       </c>
@@ -742,7 +742,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="2">
         <v>4.4000000000000004</v>
       </c>
@@ -756,7 +756,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2">
         <v>2.2999999999999998</v>
       </c>
@@ -770,7 +770,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -784,7 +784,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="2">
         <v>0.3</v>
       </c>
@@ -812,9 +812,9 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="39.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -828,7 +828,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2">
         <v>2</v>
       </c>
@@ -842,7 +842,7 @@
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2">
         <v>1.9</v>
       </c>
@@ -856,7 +856,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2">
         <v>1.7</v>
       </c>
@@ -870,7 +870,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
         <v>1.5</v>
       </c>
@@ -884,7 +884,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -898,7 +898,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
         <v>0.8</v>
       </c>
@@ -912,7 +912,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2">
         <v>0.6</v>
       </c>
@@ -926,7 +926,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="2">
         <v>0.5</v>
       </c>
@@ -953,9 +953,9 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="39.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -969,7 +969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2">
         <v>20.8</v>
       </c>
@@ -983,7 +983,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2">
         <v>19.5</v>
       </c>
@@ -997,7 +997,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2">
         <v>18.100000000000001</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
         <v>12.9</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2">
         <v>10.4</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
         <v>6.9</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2">
         <v>5</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="2">
         <v>4.4000000000000004</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="2">
         <v>2.5</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2">
         <v>1</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="2">
         <v>0.4</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="2">
         <v>0.2</v>
       </c>
@@ -1148,9 +1148,9 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="39.4" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2">
         <v>1.9</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2">
         <v>1.7</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2">
         <v>1.5</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
         <v>1.3</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
         <v>0.9</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2">
         <v>0.8</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="2">
         <v>0.5</v>
       </c>
@@ -1276,7 +1276,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="2">
         <v>0.4</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2">
         <v>0.3</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="2">
         <v>0.2</v>
       </c>
@@ -1318,7 +1318,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="2">
         <v>0.1</v>
       </c>
@@ -1345,9 +1345,9 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="26.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1358,7 +1358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2">
         <v>12.66</v>
       </c>
@@ -1369,7 +1369,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2">
         <v>12.13</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>60.6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2">
         <v>11.81</v>
       </c>
@@ -1391,7 +1391,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
         <v>12.2</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>63.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2">
         <v>16.809999999999999</v>
       </c>
@@ -1413,7 +1413,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
         <v>25.91</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2">
         <v>133.19</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>80.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="2">
         <v>53.09</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>77.2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="2">
         <v>19.100000000000001</v>
       </c>
@@ -1457,7 +1457,7 @@
         <v>66.400000000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2">
         <v>16.16</v>
       </c>
@@ -1468,7 +1468,7 @@
         <v>63.9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="2">
         <v>15.15</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>62.7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="2">
         <v>34.549999999999997</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>75.3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A14" s="2">
         <v>23.92</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>70.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="2">
         <v>17.36</v>
       </c>

</xml_diff>

<commit_message>
issues with compressor data collected now apparent
</commit_message>
<xml_diff>
--- a/IIA/3A3/Compressor_Lab/compressor_data.xlsx
+++ b/IIA/3A3/Compressor_Lab/compressor_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\source\repos\MEng-CW\IIA\3A3\Compressor_Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31C0097-85A7-4E4D-9BF7-87334EE383AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8506B252-873F-4D92-A7F2-39AB1312656A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4538" yWindow="1965" windowWidth="21599" windowHeight="11333" xr2:uid="{02A5341C-B6F3-4355-81FB-8A9D87FE953C}"/>
+    <workbookView xWindow="3360" yWindow="2932" windowWidth="21600" windowHeight="11333" activeTab="1" xr2:uid="{02A5341C-B6F3-4355-81FB-8A9D87FE953C}"/>
   </bookViews>
   <sheets>
     <sheet name="preface" sheetId="6" r:id="rId1"/>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCE3641E-77F1-44E2-8594-EE5188095FA3}">
   <dimension ref="A4:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -605,10 +605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2142626B-EBBF-4FEB-9B54-0EED73F66AB9}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -616,7 +616,7 @@
     <col min="3" max="3" width="22.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:6" ht="26.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,7 +630,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A2" s="2">
         <v>20.7</v>
       </c>
@@ -643,8 +643,12 @@
       <c r="D2" s="2">
         <v>17.899999999999999</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="F2">
+        <f>B2/(998.2*PI()*0.0252*0.0064)</f>
+        <v>1.7361791192910552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A3" s="2">
         <v>20.2</v>
       </c>
@@ -658,7 +662,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="2">
         <v>19.2</v>
       </c>
@@ -672,7 +676,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="2">
         <v>18.100000000000001</v>
       </c>
@@ -686,7 +690,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A6" s="2">
         <v>15.7</v>
       </c>
@@ -700,7 +704,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A7" s="2">
         <v>12.2</v>
       </c>
@@ -714,7 +718,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A8" s="2">
         <v>9.8000000000000007</v>
       </c>
@@ -728,7 +732,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A9" s="2">
         <v>6.6</v>
       </c>
@@ -742,7 +746,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="2">
         <v>4.4000000000000004</v>
       </c>
@@ -756,7 +760,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="2">
         <v>2.2999999999999998</v>
       </c>
@@ -770,7 +774,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -784,7 +788,7 @@
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A13" s="2">
         <v>0.3</v>
       </c>

</xml_diff>

<commit_message>
progress with the 3A3 compressor lab
</commit_message>
<xml_diff>
--- a/IIA/3A3/Compressor_Lab/compressor_data.xlsx
+++ b/IIA/3A3/Compressor_Lab/compressor_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\source\repos\MEng-CW\IIA\3A3\Compressor_Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8506B252-873F-4D92-A7F2-39AB1312656A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF9B8EE-2C35-4053-8E9B-6DE289AEF205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="2932" windowWidth="21600" windowHeight="11333" activeTab="1" xr2:uid="{02A5341C-B6F3-4355-81FB-8A9D87FE953C}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{02A5341C-B6F3-4355-81FB-8A9D87FE953C}"/>
   </bookViews>
   <sheets>
     <sheet name="preface" sheetId="6" r:id="rId1"/>
@@ -154,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -164,6 +164,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -502,7 +505,7 @@
   <dimension ref="A4:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -608,7 +611,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -630,175 +633,175 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
         <v>20.7</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.87809697639999995</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="4">
+        <v>27.76786452</v>
+      </c>
+      <c r="C2" s="4">
         <v>54.2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>17.899999999999999</v>
       </c>
       <c r="F2">
-        <f>B2/(998.2*PI()*0.0252*0.0064)</f>
-        <v>1.7361791192910552</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="2">
+        <f>B2/(998.2 * 0.0064 * 0.0252)</f>
+        <v>172.48224706256974</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="4">
         <v>20.2</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.86742711510000003</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="4">
+        <v>27.430453880000002</v>
+      </c>
+      <c r="C3" s="4">
         <v>54.3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="4">
         <v>19.2</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.84568362880000003</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="4">
+        <v>26.742864470000001</v>
+      </c>
+      <c r="C4" s="4">
         <v>55.2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="4">
         <v>18.100000000000001</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.82110102910000005</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="4">
+        <v>25.965494410000002</v>
+      </c>
+      <c r="C5" s="4">
         <v>56</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="4">
         <v>15.7</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.76472825239999997</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="4">
+        <v>24.182830689999999</v>
+      </c>
+      <c r="C6" s="4">
         <v>57.2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="4">
         <v>12.2</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.67412001899999996</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="4">
+        <v>21.317546759999999</v>
+      </c>
+      <c r="C7" s="4">
         <v>59.2</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="4">
         <v>9.8000000000000007</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.60418556749999996</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="4">
+        <v>19.10602523</v>
+      </c>
+      <c r="C8" s="4">
         <v>60.9</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="4">
         <v>6.6</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.49582597750000001</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="4">
+        <v>15.67939412</v>
+      </c>
+      <c r="C9" s="4">
         <v>62.8</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A10" s="4">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.40484021539999998</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="4">
+        <v>12.80217169</v>
+      </c>
+      <c r="C10" s="4">
         <v>63.9</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.2926989921</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="4">
+        <v>9.2559548399999994</v>
+      </c>
+      <c r="C11" s="4">
         <v>66.400000000000006</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A12" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B12" s="2">
-        <v>0.20242010769999999</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="4">
+        <v>6.4010858449999999</v>
+      </c>
+      <c r="C12" s="4">
         <v>67.099999999999994</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A13" s="4">
         <v>0.3</v>
       </c>
-      <c r="B13" s="2">
-        <v>0.1057104536</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="4">
+        <v>3.3428580590000001</v>
+      </c>
+      <c r="C13" s="4">
         <v>67.900000000000006</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="4">
         <v>17.899999999999999</v>
       </c>
     </row>
@@ -813,7 +816,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -832,115 +835,115 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.2729432175</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="4">
+        <v>8.6312223929999998</v>
+      </c>
+      <c r="C2" s="4">
         <v>16</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="4">
         <v>1.9</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.26603214089999999</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="4">
+        <v>8.4126749610000005</v>
+      </c>
+      <c r="C3" s="4">
         <v>16.2</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>18.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="4">
         <v>1.7</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.25164121280000001</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="4">
+        <v>7.957593857</v>
+      </c>
+      <c r="C4" s="4">
         <v>16.2</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>18.2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="4">
         <v>1.5</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.23637576020000001</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="4">
+        <v>7.474857858</v>
+      </c>
+      <c r="C5" s="4">
         <v>16.3</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>18.2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="4">
         <v>1</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.193</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="4">
+        <v>6.1031958839999998</v>
+      </c>
+      <c r="C6" s="4">
         <v>16.600000000000001</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>18.2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="4">
         <v>0.8</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.17262444790000001</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="4">
+        <v>5.4588643509999999</v>
+      </c>
+      <c r="C7" s="4">
         <v>16.7</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>18.2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="4">
         <v>0.6</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.14949715720000001</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="4">
+        <v>4.7275152040000004</v>
+      </c>
+      <c r="C8" s="4">
         <v>16.899999999999999</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>18.2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="4">
         <v>0.5</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.1364716088</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="4">
+        <v>4.315611197</v>
+      </c>
+      <c r="C9" s="4">
         <v>17</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>18.2</v>
       </c>
     </row>
@@ -954,7 +957,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -973,169 +976,171 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
         <v>20.8</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.88021542819999998</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="4">
+        <v>27.83485585</v>
+      </c>
+      <c r="C2" s="4">
         <v>54.6</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>18.3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="4">
         <v>19.5</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.85226492359999995</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="4">
+        <v>26.950983279999999</v>
+      </c>
+      <c r="C3" s="4">
         <v>55.7</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>18.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="4">
         <v>18.100000000000001</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.82110102910000005</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="4">
+        <v>25.965494410000002</v>
+      </c>
+      <c r="C4" s="4">
         <v>56.5</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>18.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="4">
         <v>12.9</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.69318980080000003</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="4">
+        <v>21.92058621</v>
+      </c>
+      <c r="C5" s="4">
         <v>59.6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>18.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="4">
         <v>10.4</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.62240629820000004</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="4">
+        <v>19.682215320000001</v>
+      </c>
+      <c r="C6" s="4">
         <v>61.2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>18.3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="4">
         <v>6.9</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.50696952569999998</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="4">
+        <v>16.03178406</v>
+      </c>
+      <c r="C7" s="4">
         <v>64.099999999999994</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>18.3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.4315611197</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="4">
+        <v>13.647160879999999</v>
+      </c>
+      <c r="C8" s="4">
         <v>64.599999999999994</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>18.3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="4">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.40484021539999998</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="4">
+        <v>12.80217169</v>
+      </c>
+      <c r="C9" s="4">
         <v>64.900000000000006</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>18.3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="4">
         <v>2.5</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.3051597942</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="4">
+        <v>9.65</v>
+      </c>
+      <c r="C10" s="4">
         <v>66.900000000000006</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="4">
         <v>1</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.193</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="4">
+        <v>6.1031958839999998</v>
+      </c>
+      <c r="C11" s="4">
         <v>69.099999999999994</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="4">
         <v>0.4</v>
       </c>
-      <c r="B12" s="2">
-        <v>0.1220639177</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="4">
+        <v>3.86</v>
+      </c>
+      <c r="C12" s="4">
         <v>69.900000000000006</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="4">
         <v>0.2</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="2">
+      <c r="B13" s="4">
+        <v>2.7294321749999999</v>
+      </c>
+      <c r="C13" s="4">
         <v>70</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="4">
         <v>18.5</v>
       </c>
     </row>
@@ -1148,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C1443B-01D9-4218-AEC6-94A77B7B8F5A}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1168,171 +1173,171 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="4">
         <v>1.9</v>
       </c>
-      <c r="B2" s="2">
-        <v>0.26603214089999999</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" s="4">
+        <v>8.4126749610000005</v>
+      </c>
+      <c r="C2" s="4">
         <v>16</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>18.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" s="4">
         <v>1.7</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.25164121280000001</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="4">
+        <v>7.957593857</v>
+      </c>
+      <c r="C3" s="4">
         <v>16.100000000000001</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>18.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" s="4">
         <v>1.5</v>
       </c>
-      <c r="B4" s="2">
-        <v>0.23637576020000001</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="4">
+        <v>7.474857858</v>
+      </c>
+      <c r="C4" s="4">
         <v>16.3</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>18.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" s="4">
         <v>1.3</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.22005385699999999</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="4">
+        <v>6.958713962</v>
+      </c>
+      <c r="C5" s="4">
         <v>16.5</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>18.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" s="4">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.20242010769999999</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="4">
+        <v>6.4010858449999999</v>
+      </c>
+      <c r="C6" s="4">
         <v>16.600000000000001</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>18.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" s="4">
         <v>0.9</v>
       </c>
-      <c r="B7" s="2">
-        <v>0.1830958765</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="4">
+        <v>5.79</v>
+      </c>
+      <c r="C7" s="4">
         <v>16.7</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>18.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" s="4">
         <v>0.8</v>
       </c>
-      <c r="B8" s="2">
-        <v>0.17262444790000001</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="4">
+        <v>5.4588643509999999</v>
+      </c>
+      <c r="C8" s="4">
         <v>16.7</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <v>18.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" s="4">
         <v>0.5</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.1364716088</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="B9" s="4">
+        <v>4.315611197</v>
+      </c>
+      <c r="C9" s="4">
         <v>17</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>18.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" s="4">
         <v>0.4</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.1220639177</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="4">
+        <v>3.86</v>
+      </c>
+      <c r="C10" s="4">
         <v>17.2</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="4">
         <v>18.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" s="4">
         <v>0.3</v>
       </c>
-      <c r="B11" s="2">
-        <v>0.1057104536</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="4">
+        <v>3.3428580590000001</v>
+      </c>
+      <c r="C11" s="4">
         <v>17.2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="4">
         <v>18.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" s="4">
         <v>0.2</v>
       </c>
-      <c r="B12" s="2">
-        <v>8.6312223930000001E-2</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="4">
+        <v>2.7294321749999999</v>
+      </c>
+      <c r="C12" s="4">
         <v>17.2</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="4">
         <v>18.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" s="4">
         <v>0.1</v>
       </c>
-      <c r="B13" s="2">
-        <v>6.1031958839999997E-2</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="4">
+        <v>1.93</v>
+      </c>
+      <c r="C13" s="4">
         <v>17.100000000000001</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="4">
         <v>18.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
progress with 3a3 compress
</commit_message>
<xml_diff>
--- a/IIA/3A3/Compressor_Lab/compressor_data.xlsx
+++ b/IIA/3A3/Compressor_Lab/compressor_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\louis\source\repos\MEng-CW\IIA\3A3\Compressor_Lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\MEng-CW\IIA\3A3\Compressor_Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF9B8EE-2C35-4053-8E9B-6DE289AEF205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DCB017-37E0-476F-8B1B-A49652931881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{02A5341C-B6F3-4355-81FB-8A9D87FE953C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{02A5341C-B6F3-4355-81FB-8A9D87FE953C}"/>
   </bookViews>
   <sheets>
     <sheet name="preface" sheetId="6" r:id="rId1"/>
@@ -154,7 +154,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -164,9 +164,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -505,23 +502,23 @@
   <dimension ref="A4:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="5" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -532,7 +529,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -543,7 +540,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -554,7 +551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>12</v>
       </c>
@@ -565,12 +562,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -581,8 +578,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="16" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
@@ -591,7 +588,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -608,18 +605,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2142626B-EBBF-4FEB-9B54-0EED73F66AB9}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="26.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,175 +631,190 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2" s="4">
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>20.7</v>
       </c>
-      <c r="B2" s="4">
-        <v>27.76786452</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2">
+        <v>0.87809697639999995</v>
+      </c>
+      <c r="C2" s="2">
         <v>54.2</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>17.899999999999999</v>
       </c>
       <c r="F2">
-        <f>B2/(998.2 * 0.0064 * 0.0252)</f>
-        <v>172.48224706256974</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3" s="4">
+        <f>B2/(PI() * 998.2 * 0.0064 * 0.0252)</f>
+        <v>1.7361791192910552</v>
+      </c>
+      <c r="G2">
+        <v>298.97489999999999</v>
+      </c>
+      <c r="I2">
+        <f>G2*0.0252/2</f>
+        <v>3.7670837399999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>20.2</v>
       </c>
-      <c r="B3" s="4">
-        <v>27.430453880000002</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3" s="2">
+        <v>0.86742711510000003</v>
+      </c>
+      <c r="C3" s="2">
         <v>54.3</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4" s="4">
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>19.2</v>
       </c>
-      <c r="B4" s="4">
-        <v>26.742864470000001</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="2">
+        <v>0.84568362880000003</v>
+      </c>
+      <c r="C4" s="2">
         <v>55.2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>17.899999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5" s="4">
+      <c r="I4">
+        <f>ATAN(I2/F2)</f>
+        <v>1.1389302979717717</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>18.100000000000001</v>
       </c>
-      <c r="B5" s="4">
-        <v>25.965494410000002</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" s="2">
+        <v>0.82110102910000005</v>
+      </c>
+      <c r="C5" s="2">
         <v>56</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>17.899999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6" s="4">
+      <c r="I5">
+        <f>I4*180/PI()</f>
+        <v>65.255899233359784</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>15.7</v>
       </c>
-      <c r="B6" s="4">
-        <v>24.182830689999999</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="2">
+        <v>0.76472825239999997</v>
+      </c>
+      <c r="C6" s="2">
         <v>57.2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7" s="4">
+    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>12.2</v>
       </c>
-      <c r="B7" s="4">
-        <v>21.317546759999999</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="2">
+        <v>0.67412001899999996</v>
+      </c>
+      <c r="C7" s="2">
         <v>59.2</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A8" s="4">
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>9.8000000000000007</v>
       </c>
-      <c r="B8" s="4">
-        <v>19.10602523</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" s="2">
+        <v>0.60418556749999996</v>
+      </c>
+      <c r="C8" s="2">
         <v>60.9</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A9" s="4">
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>6.6</v>
       </c>
-      <c r="B9" s="4">
-        <v>15.67939412</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="2">
+        <v>0.49582597750000001</v>
+      </c>
+      <c r="C9" s="2">
         <v>62.8</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A10" s="4">
+    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B10" s="4">
-        <v>12.80217169</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="2">
+        <v>0.40484021539999998</v>
+      </c>
+      <c r="C10" s="2">
         <v>63.9</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="2">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A11" s="4">
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="B11" s="4">
-        <v>9.2559548399999994</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" s="2">
+        <v>0.2926989921</v>
+      </c>
+      <c r="C11" s="2">
         <v>66.400000000000006</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="2">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A12" s="4">
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B12" s="4">
-        <v>6.4010858449999999</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="B12" s="2">
+        <v>0.20242010769999999</v>
+      </c>
+      <c r="C12" s="2">
         <v>67.099999999999994</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <v>17.899999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A13" s="4">
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>0.3</v>
       </c>
-      <c r="B13" s="4">
-        <v>3.3428580590000001</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B13" s="2">
+        <v>0.1057104536</v>
+      </c>
+      <c r="C13" s="2">
         <v>67.900000000000006</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="2">
         <v>17.899999999999999</v>
       </c>
     </row>
@@ -816,12 +829,12 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D9" sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -835,115 +848,115 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="4">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>2</v>
       </c>
-      <c r="B2" s="4">
-        <v>8.6312223929999998</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2">
+        <v>0.2729432175</v>
+      </c>
+      <c r="C2" s="2">
         <v>16</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>18.100000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="4">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>1.9</v>
       </c>
-      <c r="B3" s="4">
-        <v>8.4126749610000005</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3" s="2">
+        <v>0.26603214089999999</v>
+      </c>
+      <c r="C3" s="2">
         <v>16.2</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>18.2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="4">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>1.7</v>
       </c>
-      <c r="B4" s="4">
-        <v>7.957593857</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="2">
+        <v>0.25164121280000001</v>
+      </c>
+      <c r="C4" s="2">
         <v>16.2</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>18.2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="4">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>1.5</v>
       </c>
-      <c r="B5" s="4">
-        <v>7.474857858</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" s="2">
+        <v>0.23637576020000001</v>
+      </c>
+      <c r="C5" s="2">
         <v>16.3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>18.2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="4">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="4">
-        <v>6.1031958839999998</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="2">
+        <v>0.193</v>
+      </c>
+      <c r="C6" s="2">
         <v>16.600000000000001</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>18.2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="4">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>0.8</v>
       </c>
-      <c r="B7" s="4">
-        <v>5.4588643509999999</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="2">
+        <v>0.17262444790000001</v>
+      </c>
+      <c r="C7" s="2">
         <v>16.7</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>18.2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="4">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>0.6</v>
       </c>
-      <c r="B8" s="4">
-        <v>4.7275152040000004</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" s="2">
+        <v>0.14949715720000001</v>
+      </c>
+      <c r="C8" s="2">
         <v>16.899999999999999</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>18.2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="4">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>0.5</v>
       </c>
-      <c r="B9" s="4">
-        <v>4.315611197</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="2">
+        <v>0.1364716088</v>
+      </c>
+      <c r="C9" s="2">
         <v>17</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <v>18.2</v>
       </c>
     </row>
@@ -957,12 +970,12 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D13" sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -976,171 +989,171 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="4">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>20.8</v>
       </c>
-      <c r="B2" s="4">
-        <v>27.83485585</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2">
+        <v>0.88021542819999998</v>
+      </c>
+      <c r="C2" s="2">
         <v>54.6</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>18.3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="4">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>19.5</v>
       </c>
-      <c r="B3" s="4">
-        <v>26.950983279999999</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3" s="2">
+        <v>0.85226492359999995</v>
+      </c>
+      <c r="C3" s="2">
         <v>55.7</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>18.3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="4">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>18.100000000000001</v>
       </c>
-      <c r="B4" s="4">
-        <v>25.965494410000002</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="2">
+        <v>0.82110102910000005</v>
+      </c>
+      <c r="C4" s="2">
         <v>56.5</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>18.3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="4">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>12.9</v>
       </c>
-      <c r="B5" s="4">
-        <v>21.92058621</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" s="2">
+        <v>0.69318980080000003</v>
+      </c>
+      <c r="C5" s="2">
         <v>59.6</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>18.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="4">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>10.4</v>
       </c>
-      <c r="B6" s="4">
-        <v>19.682215320000001</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="2">
+        <v>0.62240629820000004</v>
+      </c>
+      <c r="C6" s="2">
         <v>61.2</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>18.3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="4">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>6.9</v>
       </c>
-      <c r="B7" s="4">
-        <v>16.03178406</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="2">
+        <v>0.50696952569999998</v>
+      </c>
+      <c r="C7" s="2">
         <v>64.099999999999994</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>18.3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="4">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="4">
-        <v>13.647160879999999</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" s="2">
+        <v>0.4315611197</v>
+      </c>
+      <c r="C8" s="2">
         <v>64.599999999999994</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>18.3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="4">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="B9" s="4">
-        <v>12.80217169</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="2">
+        <v>0.40484021539999998</v>
+      </c>
+      <c r="C9" s="2">
         <v>64.900000000000006</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <v>18.3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="4">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>2.5</v>
       </c>
-      <c r="B10" s="4">
-        <v>9.65</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="2">
+        <v>0.3051597942</v>
+      </c>
+      <c r="C10" s="2">
         <v>66.900000000000006</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="2">
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="4">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B11" s="4">
-        <v>6.1031958839999998</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" s="2">
+        <v>0.193</v>
+      </c>
+      <c r="C11" s="2">
         <v>69.099999999999994</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="2">
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="4">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>0.4</v>
       </c>
-      <c r="B12" s="4">
-        <v>3.86</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="B12" s="2">
+        <v>0.1220639177</v>
+      </c>
+      <c r="C12" s="2">
         <v>69.900000000000006</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="4">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>0.2</v>
       </c>
-      <c r="B13" s="4">
-        <v>2.7294321749999999</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B13" s="2">
+        <v>8.6312223930000001E-2</v>
+      </c>
+      <c r="C13" s="2">
         <v>70</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="2">
         <v>18.5</v>
       </c>
     </row>
@@ -1153,13 +1166,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4C1443B-01D9-4218-AEC6-94A77B7B8F5A}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="39.4" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1173,171 +1186,171 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="4">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1.9</v>
       </c>
-      <c r="B2" s="4">
-        <v>8.4126749610000005</v>
-      </c>
-      <c r="C2" s="4">
+      <c r="B2" s="2">
+        <v>0.26603214089999999</v>
+      </c>
+      <c r="C2" s="2">
         <v>16</v>
       </c>
-      <c r="D2" s="4">
+      <c r="D2" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="4">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>1.7</v>
       </c>
-      <c r="B3" s="4">
-        <v>7.957593857</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3" s="2">
+        <v>0.25164121280000001</v>
+      </c>
+      <c r="C3" s="2">
         <v>16.100000000000001</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="4">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>1.5</v>
       </c>
-      <c r="B4" s="4">
-        <v>7.474857858</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="2">
+        <v>0.23637576020000001</v>
+      </c>
+      <c r="C4" s="2">
         <v>16.3</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="4">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>1.3</v>
       </c>
-      <c r="B5" s="4">
-        <v>6.958713962</v>
-      </c>
-      <c r="C5" s="4">
+      <c r="B5" s="2">
+        <v>0.22005385699999999</v>
+      </c>
+      <c r="C5" s="2">
         <v>16.5</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="4">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B6" s="4">
-        <v>6.4010858449999999</v>
-      </c>
-      <c r="C6" s="4">
+      <c r="B6" s="2">
+        <v>0.20242010769999999</v>
+      </c>
+      <c r="C6" s="2">
         <v>16.600000000000001</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="4">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>0.9</v>
       </c>
-      <c r="B7" s="4">
-        <v>5.79</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="2">
+        <v>0.1830958765</v>
+      </c>
+      <c r="C7" s="2">
         <v>16.7</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="4">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>0.8</v>
       </c>
-      <c r="B8" s="4">
-        <v>5.4588643509999999</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" s="2">
+        <v>0.17262444790000001</v>
+      </c>
+      <c r="C8" s="2">
         <v>16.7</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="4">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>0.5</v>
       </c>
-      <c r="B9" s="4">
-        <v>4.315611197</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="2">
+        <v>0.1364716088</v>
+      </c>
+      <c r="C9" s="2">
         <v>17</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="4">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>0.4</v>
       </c>
-      <c r="B10" s="4">
-        <v>3.86</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="2">
+        <v>0.1220639177</v>
+      </c>
+      <c r="C10" s="2">
         <v>17.2</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="4">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>0.3</v>
       </c>
-      <c r="B11" s="4">
-        <v>3.3428580590000001</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" s="2">
+        <v>0.1057104536</v>
+      </c>
+      <c r="C11" s="2">
         <v>17.2</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="4">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>0.2</v>
       </c>
-      <c r="B12" s="4">
-        <v>2.7294321749999999</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="B12" s="2">
+        <v>8.6312223930000001E-2</v>
+      </c>
+      <c r="C12" s="2">
         <v>17.2</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="2">
         <v>18.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="4">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>0.1</v>
       </c>
-      <c r="B13" s="4">
-        <v>1.93</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B13" s="2">
+        <v>6.1031958839999997E-2</v>
+      </c>
+      <c r="C13" s="2">
         <v>17.100000000000001</v>
       </c>
-      <c r="D13" s="4">
+      <c r="D13" s="2">
         <v>18.5</v>
       </c>
     </row>
@@ -1350,13 +1363,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A75AFA-7BB2-4C2C-B496-6CA4110F020A}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1367,7 +1380,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>12.66</v>
       </c>
@@ -1378,7 +1391,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>12.13</v>
       </c>
@@ -1389,7 +1402,7 @@
         <v>60.6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>11.81</v>
       </c>
@@ -1400,7 +1413,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>12.2</v>
       </c>
@@ -1411,7 +1424,7 @@
         <v>63.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>16.809999999999999</v>
       </c>
@@ -1422,7 +1435,7 @@
         <v>68.7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>25.91</v>
       </c>
@@ -1433,7 +1446,7 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>133.19</v>
       </c>
@@ -1444,7 +1457,7 @@
         <v>80.5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>53.09</v>
       </c>
@@ -1455,7 +1468,7 @@
         <v>77.2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>19.100000000000001</v>
       </c>
@@ -1466,7 +1479,7 @@
         <v>66.400000000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>16.16</v>
       </c>
@@ -1477,7 +1490,7 @@
         <v>63.9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>15.15</v>
       </c>
@@ -1488,7 +1501,7 @@
         <v>62.7</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>34.549999999999997</v>
       </c>
@@ -1499,7 +1512,7 @@
         <v>75.3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>23.92</v>
       </c>
@@ -1510,7 +1523,7 @@
         <v>70.5</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>17.36</v>
       </c>

</xml_diff>

<commit_message>
uhm this should have been in the last commit
</commit_message>
<xml_diff>
--- a/IIA/3A3/Compressor_Lab/compressor_data.xlsx
+++ b/IIA/3A3/Compressor_Lab/compressor_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\MEng-CW\IIA\3A3\Compressor_Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DCB017-37E0-476F-8B1B-A49652931881}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCDDB80-9E6A-4D9F-872D-6173E3607F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{02A5341C-B6F3-4355-81FB-8A9D87FE953C}"/>
   </bookViews>
@@ -608,7 +608,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,8 +645,8 @@
         <v>17.899999999999999</v>
       </c>
       <c r="F2">
-        <f>B2/(PI() * 998.2 * 0.0064 * 0.0252)</f>
-        <v>1.7361791192910552</v>
+        <f>B2/(PI() * 998.2 * 0.0064 * 0.0252 - 2 *6 * 0.0039)</f>
+        <v>1.9132151713422394</v>
       </c>
       <c r="G2">
         <v>298.97489999999999</v>
@@ -685,7 +685,7 @@
       </c>
       <c r="I4">
         <f>ATAN(I2/F2)</f>
-        <v>1.1389302979717717</v>
+        <v>1.1008669967855766</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -703,7 +703,7 @@
       </c>
       <c r="I5">
         <f>I4*180/PI()</f>
-        <v>65.255899233359784</v>
+        <v>63.075032721055507</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -829,7 +829,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="A1:D9"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>